<commit_message>
update testing function v2
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -8,12 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Fpoly_HCM\SOF3012_LapTrinh-JAVA4\sof3012-assignment-java4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BD33253-7245-4DD9-B7F2-7674AB9F2A9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45BB251B-4B50-4DBB-B2D7-2E1474434765}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{B44DAD84-7207-408B-934D-2EB6900F3E91}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="8" xr2:uid="{B44DAD84-7207-408B-934D-2EB6900F3E91}"/>
   </bookViews>
   <sheets>
-    <sheet name="LoginData" sheetId="1" r:id="rId1"/>
+    <sheet name="UserFind" sheetId="1" r:id="rId1"/>
+    <sheet name="UserCreate" sheetId="3" r:id="rId2"/>
+    <sheet name="UserUpdate" sheetId="4" r:id="rId3"/>
+    <sheet name="UserDelete" sheetId="5" r:id="rId4"/>
+    <sheet name="Login" sheetId="6" r:id="rId5"/>
+    <sheet name="VideoCreate" sheetId="7" r:id="rId6"/>
+    <sheet name="VideoFind" sheetId="8" r:id="rId7"/>
+    <sheet name="VideoUpdate" sheetId="9" r:id="rId8"/>
+    <sheet name="VideoDelete" sheetId="10" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,37 +44,208 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
-  <si>
-    <t>Username</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>ExpectedStatus</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="65">
   <si>
     <t>admin</t>
   </si>
   <si>
-    <t>Pass</t>
-  </si>
-  <si>
-    <t>sai_pass_roi</t>
-  </si>
-  <si>
-    <t>Fail</t>
-  </si>
-  <si>
-    <t>user_ma_la</t>
+    <t>TC_ID</t>
+  </si>
+  <si>
+    <t>INPUT_ID</t>
+  </si>
+  <si>
+    <t>EXPECTED</t>
+  </si>
+  <si>
+    <t>TC_FIND_01</t>
+  </si>
+  <si>
+    <t>TC_FIND_02</t>
+  </si>
+  <si>
+    <t>TC_FIND_03</t>
+  </si>
+  <si>
+    <t>xyz</t>
+  </si>
+  <si>
+    <t>NOT_NULL</t>
+  </si>
+  <si>
+    <t>NULL</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>NAME</t>
+  </si>
+  <si>
+    <t>EMAIL</t>
+  </si>
+  <si>
+    <t>TC_CREATE_04</t>
+  </si>
+  <si>
+    <t>TC_CREATE_05</t>
+  </si>
+  <si>
+    <t>TC_CREATE_06</t>
+  </si>
+  <si>
+    <t>TC_CREATE_07</t>
+  </si>
+  <si>
+    <t>new01</t>
+  </si>
+  <si>
+    <t>NULL_VAL</t>
+  </si>
+  <si>
+    <t>new02</t>
+  </si>
+  <si>
+    <t>New User</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>Ghost</t>
+  </si>
+  <si>
+    <t>No Email</t>
+  </si>
+  <si>
+    <t>n@a.com</t>
+  </si>
+  <si>
+    <t>a@a.com</t>
+  </si>
+  <si>
+    <t>g@a.com</t>
+  </si>
+  <si>
+    <t>SUCCESS</t>
+  </si>
+  <si>
+    <t>DUPLICATE</t>
+  </si>
+  <si>
+    <t>ERROR</t>
+  </si>
+  <si>
+    <t>NEW_NAME</t>
+  </si>
+  <si>
+    <t>TC_UPDATE_08</t>
+  </si>
+  <si>
+    <t>TC_UPDATE_09</t>
+  </si>
+  <si>
+    <t>ghost</t>
+  </si>
+  <si>
+    <t>Admin Updated</t>
+  </si>
+  <si>
+    <t>TC_DELETE_10</t>
+  </si>
+  <si>
+    <t>TC_DELETE_11</t>
+  </si>
+  <si>
+    <t>USERNAME</t>
+  </si>
+  <si>
+    <t>PASSWORD</t>
+  </si>
+  <si>
+    <t>TC_LOGIN_12</t>
+  </si>
+  <si>
+    <t>TC_LOGIN_13</t>
+  </si>
+  <si>
+    <t>TC_LOGIN_14</t>
+  </si>
+  <si>
+    <t>TC_LOGIN_15</t>
+  </si>
+  <si>
+    <t>TC_LOGIN_16</t>
+  </si>
+  <si>
+    <t>kocos</t>
+  </si>
+  <si>
+    <t>sai</t>
+  </si>
+  <si>
+    <t>EMPTY_USER</t>
+  </si>
+  <si>
+    <t>EMPTY_PASS</t>
+  </si>
+  <si>
+    <t>WRONG_PASS</t>
+  </si>
+  <si>
+    <t>WRONG_USER</t>
+  </si>
+  <si>
+    <t>TC_CREATE_17</t>
+  </si>
+  <si>
+    <t>TC_CREATE_18</t>
+  </si>
+  <si>
+    <t>TC_CREATE_19</t>
+  </si>
+  <si>
+    <t>v01</t>
+  </si>
+  <si>
+    <t>v02</t>
+  </si>
+  <si>
+    <t>TITLE</t>
+  </si>
+  <si>
+    <t>Java 2</t>
+  </si>
+  <si>
+    <t>Java 1</t>
+  </si>
+  <si>
+    <t>TC_FIND_20</t>
+  </si>
+  <si>
+    <t>NEW_TITLE</t>
+  </si>
+  <si>
+    <t>TC_UPDATE_21</t>
+  </si>
+  <si>
+    <t>Java Adv</t>
+  </si>
+  <si>
+    <t>TC_DELETE_22</t>
+  </si>
+  <si>
+    <t>FK_ERROR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -80,6 +259,29 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -89,7 +291,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -97,35 +299,47 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFCCCCCC"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFCCCCCC"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFCCCCCC"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FFCCCCCC"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -458,70 +672,640 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18885609-FA9B-4412-8CF0-0F8043EA669D}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.140625" customWidth="1"/>
-    <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="20" style="5" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" style="5" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C2" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D915BBD7-6FE2-45CF-AC51-7637B9334D02}">
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.140625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="20" style="5" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="17" style="5" customWidth="1"/>
+    <col min="6" max="6" width="18.28515625" style="5" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="10">
         <v>123</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+      <c r="D2" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="10">
+        <v>123</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="10">
+        <v>123</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="10">
+        <v>123</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E4" r:id="rId1" xr:uid="{030C5789-244C-42F4-9FAD-E99EC9965DD5}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{B0291E61-CFBD-4BC5-8AD1-54304DC0C696}"/>
+    <hyperlink ref="E2" r:id="rId3" xr:uid="{48579166-00F8-499B-BFA9-9F600DE5A6FF}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC879374-BA74-4E65-B0B5-E8AC5B03ECB5}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.140625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="20" style="5" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="17" style="5" customWidth="1"/>
+    <col min="6" max="6" width="18.28515625" style="5" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="1">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93A47FDA-B862-451A-A988-F0F358C756AB}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.140625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="20" style="5" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="17" style="5" customWidth="1"/>
+    <col min="6" max="6" width="18.28515625" style="5" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AA36775-0B5B-4B8E-888B-7A474C504363}">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.140625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="20" style="5" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="17" style="5" customWidth="1"/>
+    <col min="6" max="6" width="18.28515625" style="5" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="8">
         <v>123</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1">
+      <c r="D2" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="8">
         <v>123</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>6</v>
+      <c r="D4" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8">
+        <v>123</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04908270-5C5D-4B79-89D3-4A643B032BA3}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.140625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="20" style="5" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="17" style="5" customWidth="1"/>
+    <col min="6" max="6" width="18.28515625" style="5" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE72E36E-8CFC-4415-B95F-8AEACD14ADDE}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.140625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="20" style="5" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="17" style="5" customWidth="1"/>
+    <col min="6" max="6" width="18.28515625" style="5" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62106DD3-8978-4B20-99D5-CA3A00AFCF04}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.140625" style="5" customWidth="1"/>
+    <col min="2" max="3" width="20" style="5" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="17" style="5" customWidth="1"/>
+    <col min="7" max="7" width="18.28515625" style="5" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F43B5D8F-98E7-49B9-B72B-E1ECAA15B8DB}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.140625" style="5" customWidth="1"/>
+    <col min="2" max="3" width="20" style="5" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="17" style="5" customWidth="1"/>
+    <col min="7" max="7" width="18.28515625" style="5" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update testing function v3
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Fpoly_HCM\SOF3012_LapTrinh-JAVA4\sof3012-assignment-java4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45BB251B-4B50-4DBB-B2D7-2E1474434765}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2AE3ED1-625A-4943-91A2-478BF67C0DFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="8" xr2:uid="{B44DAD84-7207-408B-934D-2EB6900F3E91}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="64">
   <si>
     <t>admin</t>
   </si>
@@ -236,9 +236,6 @@
   </si>
   <si>
     <t>TC_DELETE_22</t>
-  </si>
-  <si>
-    <t>FK_ERROR</t>
   </si>
 </sst>
 </file>
@@ -304,22 +301,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -330,9 +327,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -773,19 +767,19 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="6" t="s">
         <v>14</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="10">
+      <c r="C2" s="6">
         <v>123</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="10" t="s">
         <v>25</v>
       </c>
       <c r="F2" s="2" t="s">
@@ -793,19 +787,19 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="10">
+      <c r="C3" s="6">
         <v>123</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="10" t="s">
         <v>26</v>
       </c>
       <c r="F3" s="6" t="s">
@@ -813,42 +807,42 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4" s="6">
         <v>123</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="E4" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="6" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C5" s="6">
         <v>123</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="F5" s="6" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1272,7 +1266,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -1305,7 +1299,7 @@
         <v>54</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>64</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>